<commit_message>
Typo on Shakespeare spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheets/Chapter04-Shakespeare-model.xlsx
+++ b/spreadsheets/Chapter04-Shakespeare-model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stout\Google Drive\__Projetos\__TODO\Books-writing\2022\Markov Chains primer\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C7F62D-F357-40ED-B541-EAE6F4AC34AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73833C0-D04E-47B0-B96C-184D6AAA6CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EC5795B-E84C-4786-A20A-5069F0C12260}"/>
   </bookViews>
@@ -166,7 +166,7 @@
     <t>word</t>
   </si>
   <si>
-    <t>CLEARING PONCTUATION AND OTHER CHARACTERS</t>
+    <t>CLEARING PUNCTUATION AND OTHER CHARACTERS</t>
   </si>
 </sst>
 </file>
@@ -49710,79 +49710,79 @@
       </c>
       <c r="J511">
         <f ca="1">RAND()</f>
-        <v>0.55869061364028594</v>
+        <v>0.52949290045482933</v>
       </c>
       <c r="K511">
         <f t="shared" ref="K511:AB511" ca="1" si="42">RAND()</f>
-        <v>3.690386293701331E-2</v>
+        <v>0.2609201617301895</v>
       </c>
       <c r="L511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.22766084108987694</v>
+        <v>0.12492062782700153</v>
       </c>
       <c r="M511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.40643715231803923</v>
+        <v>0.97347179401534933</v>
       </c>
       <c r="N511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.59955708383711437</v>
+        <v>0.95720978310278648</v>
       </c>
       <c r="O511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.94472362010796684</v>
+        <v>0.60752408635438537</v>
       </c>
       <c r="P511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.89406857713518439</v>
+        <v>0.28471803591422218</v>
       </c>
       <c r="Q511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.50451541218714224</v>
+        <v>1.9937036586432866E-2</v>
       </c>
       <c r="R511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.44337516576790892</v>
+        <v>0.86010141123490236</v>
       </c>
       <c r="S511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.53260166436652767</v>
+        <v>0.37057804450505627</v>
       </c>
       <c r="T511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.23949993491934984</v>
+        <v>1.1122869697224202E-2</v>
       </c>
       <c r="U511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.50600941244095021</v>
+        <v>0.24290592507133446</v>
       </c>
       <c r="V511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.81851876270161117</v>
+        <v>0.88218158958564585</v>
       </c>
       <c r="W511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.36024450637440597</v>
+        <v>0.8158426679373203</v>
       </c>
       <c r="X511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.74668814722838295</v>
+        <v>0.65009469780383689</v>
       </c>
       <c r="Y511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.70355763063194443</v>
+        <v>0.78299953713155834</v>
       </c>
       <c r="Z511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.48655843196476556</v>
+        <v>8.4325318722444198E-2</v>
       </c>
       <c r="AA511">
         <f t="shared" ca="1" si="42"/>
-        <v>5.9338880321061271E-2</v>
+        <v>7.6812600139771092E-2</v>
       </c>
       <c r="AB511">
         <f t="shared" ca="1" si="42"/>
-        <v>0.67666322852480076</v>
+        <v>7.8376780180075212E-2</v>
       </c>
     </row>
     <row r="512" spans="2:28" x14ac:dyDescent="0.3">
@@ -49838,7 +49838,7 @@
       </c>
       <c r="Q512" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>a</v>
       </c>
       <c r="R512" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -49850,7 +49850,7 @@
       </c>
       <c r="T512" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>a</v>
       </c>
       <c r="U512" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -49914,7 +49914,7 @@
       </c>
       <c r="K513" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>b</v>
+        <v/>
       </c>
       <c r="L513" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50078,7 +50078,7 @@
       </c>
       <c r="AA514" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>c</v>
+        <v/>
       </c>
       <c r="AB514" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50118,7 +50118,7 @@
       </c>
       <c r="L515" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>d</v>
       </c>
       <c r="M515" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50174,15 +50174,15 @@
       </c>
       <c r="Z515" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>d</v>
       </c>
       <c r="AA515" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>d</v>
       </c>
       <c r="AB515" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>d</v>
       </c>
     </row>
     <row r="516" spans="2:28" x14ac:dyDescent="0.3">
@@ -50318,7 +50318,7 @@
       </c>
       <c r="L517" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>f</v>
+        <v/>
       </c>
       <c r="M517" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50350,11 +50350,11 @@
       </c>
       <c r="T517" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>f</v>
+        <v/>
       </c>
       <c r="U517" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>f</v>
       </c>
       <c r="V517" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50414,7 +50414,7 @@
       </c>
       <c r="K518" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>g</v>
       </c>
       <c r="L518" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50434,7 +50434,7 @@
       </c>
       <c r="P518" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>g</v>
       </c>
       <c r="Q518" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50746,7 +50746,7 @@
       </c>
       <c r="S521" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v/>
+        <v>j</v>
       </c>
       <c r="T521" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50762,7 +50762,7 @@
       </c>
       <c r="W521" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>j</v>
+        <v/>
       </c>
       <c r="X521" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -50922,7 +50922,7 @@
       </c>
       <c r="M523" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>l</v>
+        <v/>
       </c>
       <c r="N523" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -51042,7 +51042,7 @@
       </c>
       <c r="R524" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>m</v>
+        <v/>
       </c>
       <c r="S524" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -51138,7 +51138,7 @@
       </c>
       <c r="Q525" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>n</v>
+        <v/>
       </c>
       <c r="R525" t="str">
         <f t="shared" ref="R525:AB536" ca="1" si="46">IF(AND(R$511&gt;$G524,R$511&lt;=$H524),$E524,"")</f>
@@ -51154,7 +51154,7 @@
       </c>
       <c r="U525" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>n</v>
+        <v/>
       </c>
       <c r="V525" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51174,7 +51174,7 @@
       </c>
       <c r="Z525" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>n</v>
+        <v/>
       </c>
       <c r="AA525" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51210,7 +51210,7 @@
       </c>
       <c r="J526" t="str">
         <f t="shared" ref="J526:Q536" ca="1" si="47">IF(AND(J$511&gt;$G525,J$511&lt;=$H525),$E525,"")</f>
-        <v/>
+        <v>o</v>
       </c>
       <c r="K526" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -51246,7 +51246,7 @@
       </c>
       <c r="S526" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>o</v>
+        <v/>
       </c>
       <c r="T526" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51310,7 +51310,7 @@
       </c>
       <c r="J527" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v>p</v>
+        <v/>
       </c>
       <c r="K527" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -51526,11 +51526,11 @@
       </c>
       <c r="N529" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v>r</v>
+        <v/>
       </c>
       <c r="O529" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v/>
+        <v>r</v>
       </c>
       <c r="P529" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -51666,7 +51666,7 @@
       </c>
       <c r="X530" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>s</v>
       </c>
       <c r="Y530" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51682,7 +51682,7 @@
       </c>
       <c r="AB530" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>s</v>
+        <v/>
       </c>
     </row>
     <row r="531" spans="2:28" x14ac:dyDescent="0.3">
@@ -51770,7 +51770,7 @@
       </c>
       <c r="Y531" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>t</v>
+        <v/>
       </c>
       <c r="Z531" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51866,7 +51866,7 @@
       </c>
       <c r="X532" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Y532" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -51970,7 +51970,7 @@
       </c>
       <c r="Y533" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>v</v>
       </c>
       <c r="Z533" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -52058,11 +52058,11 @@
       </c>
       <c r="V534" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>w</v>
+        <v/>
       </c>
       <c r="W534" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>w</v>
       </c>
       <c r="X534" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -52134,7 +52134,7 @@
       </c>
       <c r="P535" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v>x</v>
+        <v/>
       </c>
       <c r="Q535" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -52142,7 +52142,7 @@
       </c>
       <c r="R535" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="S535" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -52158,7 +52158,7 @@
       </c>
       <c r="V535" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>x</v>
       </c>
       <c r="W535" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -52226,11 +52226,11 @@
       </c>
       <c r="N536" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v/>
+        <v>y</v>
       </c>
       <c r="O536" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v>y</v>
+        <v/>
       </c>
       <c r="P536" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -52297,79 +52297,79 @@
       </c>
       <c r="J537" s="5" t="str">
         <f ca="1">_xlfn.CONCAT(J512:J536)</f>
-        <v>p</v>
+        <v>o</v>
       </c>
       <c r="K537" s="5" t="str">
         <f t="shared" ref="K537:AB537" ca="1" si="48">_xlfn.CONCAT(K512:K536)</f>
-        <v>b</v>
+        <v>g</v>
       </c>
       <c r="L537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>f</v>
+        <v>d</v>
       </c>
       <c r="M537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>l</v>
+        <v/>
       </c>
       <c r="N537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>r</v>
+        <v>y</v>
       </c>
       <c r="O537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>y</v>
+        <v>r</v>
       </c>
       <c r="P537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>x</v>
+        <v>g</v>
       </c>
       <c r="Q537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>n</v>
+        <v>a</v>
       </c>
       <c r="R537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>m</v>
+        <v>x</v>
       </c>
       <c r="S537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>o</v>
+        <v>j</v>
       </c>
       <c r="T537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>f</v>
+        <v>a</v>
       </c>
       <c r="U537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>n</v>
+        <v>f</v>
       </c>
       <c r="V537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>w</v>
+        <v>x</v>
       </c>
       <c r="W537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>j</v>
+        <v>w</v>
       </c>
       <c r="X537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>u</v>
+        <v>s</v>
       </c>
       <c r="Y537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>t</v>
+        <v>v</v>
       </c>
       <c r="Z537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>n</v>
+        <v>d</v>
       </c>
       <c r="AA537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>c</v>
+        <v>d</v>
       </c>
       <c r="AB537" s="5" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>s</v>
+        <v>d</v>
       </c>
     </row>
     <row r="538" spans="2:28" x14ac:dyDescent="0.3">
@@ -52384,7 +52384,7 @@
       </c>
       <c r="J538" s="5" t="str">
         <f ca="1">_xlfn.CONCAT(J537:AB537)</f>
-        <v>pbflryxnmofnwjutncs</v>
+        <v>ogdyrgaxjafxwsvddd</v>
       </c>
       <c r="K538" s="5"/>
       <c r="L538" s="5"/>

</xml_diff>